<commit_message>
Update BDC_Locations of Files,Settings&DBsUsed.xlsx
</commit_message>
<xml_diff>
--- a/BDC_V1/Documents/BDC_Locations of Files,Settings&DBsUsed.xlsx
+++ b/BDC_V1/Documents/BDC_Locations of Files,Settings&DBsUsed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill_\source\Projects\BDC\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA54F6A0-966B-4F5C-83D1-3BE6A1448AB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8374B41D-1F08-4D66-9986-7004241BBC34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23310" yWindow="2925" windowWidth="23640" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26355" yWindow="1680" windowWidth="23640" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files &amp; Locations" sheetId="1" r:id="rId1"/>
@@ -563,9 +563,6 @@
     <t>BDC Error &amp; Trace Logs Folder</t>
   </si>
   <si>
-    <t>C:\Users\&lt;USER&gt;\AppData\BuilderDC\Logs</t>
-  </si>
-  <si>
     <t>FileUserCache</t>
   </si>
   <si>
@@ -594,6 +591,9 @@
   </si>
   <si>
     <t>on-demand</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;UserName&gt;\AppData\Roaming\BuilderDC\Logs</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2009,7 +2009,7 @@
         <v>121</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>17</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>55</v>
@@ -2108,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>112</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>103</v>
@@ -2131,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>111</v>
@@ -2244,7 +2244,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G24" s="19" t="s">
         <v>112</v>
@@ -2267,7 +2267,7 @@
         <v>16</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>112</v>
@@ -2313,7 +2313,7 @@
         <v>17</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>112</v>
@@ -2359,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" s="19" t="s">
         <v>112</v>
@@ -2382,7 +2382,7 @@
         <v>16</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>112</v>
@@ -2405,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>112</v>
@@ -2428,7 +2428,7 @@
         <v>16</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G32" s="19" t="s">
         <v>112</v>
@@ -2451,7 +2451,7 @@
         <v>16</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G33" s="19" t="s">
         <v>112</v>

</xml_diff>